<commit_message>
Unexpected Result From Background Process
</commit_message>
<xml_diff>
--- a/aplicacionesResumen.xlsx
+++ b/aplicacionesResumen.xlsx
@@ -555,7 +555,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:C16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -707,7 +707,7 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Browser Embedded Incorrectly diseñada
</commit_message>
<xml_diff>
--- a/aplicacionesResumen.xlsx
+++ b/aplicacionesResumen.xlsx
@@ -156,18 +156,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Source Sans Pro"/>
     </font>
     <font>
       <sz val="11"/>
@@ -220,16 +215,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -555,10 +547,10 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
@@ -569,21 +561,21 @@
     <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -591,137 +583,137 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="84" customHeight="1">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43.5">
-      <c r="A18" t="s">
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="6" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Unclear Behavior casi terminada. Comentario en el excel
</commit_message>
<xml_diff>
--- a/aplicacionesResumen.xlsx
+++ b/aplicacionesResumen.xlsx
@@ -23,6 +23,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Michael Stiven Osorio Riaño</author>
+  </authors>
+  <commentList>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{55D12E5E-0BFC-4DD7-A421-46D9BE6FC3E9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Stiven Osorio Riaño:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+faltan algunos arreglos pero ya está casi terminada. El getItemCount() siempre es 0</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
@@ -156,7 +190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +203,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -543,11 +590,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CF7B7E-78AD-4E97-B126-25CCD3E733F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CF7B7E-78AD-4E97-B126-25CCD3E733F2}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:D18"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +650,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -720,5 +767,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Redirection without connectivity check terminada
</commit_message>
<xml_diff>
--- a/aplicacionesResumen.xlsx
+++ b/aplicacionesResumen.xlsx
@@ -621,7 +621,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,13 +746,13 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nonexistent notification of progres while downloading content terminada
</commit_message>
<xml_diff>
--- a/aplicacionesResumen.xlsx
+++ b/aplicacionesResumen.xlsx
@@ -621,7 +621,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +707,7 @@
       <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -723,10 +723,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="6" t="s">

</xml_diff>